<commit_message>
terminar histograma, analise grafica e conclusão.
</commit_message>
<xml_diff>
--- a/EXP_3/Tabelas_EXP_3.xlsx
+++ b/EXP_3/Tabelas_EXP_3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre Filho\Documents\FISICA_1\EXP_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8458BF6C-89EC-4A30-8E53-E411D93905E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6FA7A1-4087-4D1D-A730-813748BA3AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1CF05FF6-7035-4474-8161-1C2C7AE69166}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Medidas</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Tempo (s)3</t>
   </si>
   <si>
-    <t>Medidas4</t>
-  </si>
-  <si>
     <t>Tempo (s)5</t>
   </si>
   <si>
@@ -85,15 +82,9 @@
     <t>128cm</t>
   </si>
   <si>
-    <t>138cm</t>
-  </si>
-  <si>
     <t>118cm</t>
   </si>
   <si>
-    <t>158cm</t>
-  </si>
-  <si>
     <t>Experimento 3 - Plano Inclinado</t>
   </si>
   <si>
@@ -217,22 +208,7 @@
     <t>0.1266</t>
   </si>
   <si>
-    <t>0.1216</t>
-  </si>
-  <si>
-    <t>0.1214</t>
-  </si>
-  <si>
-    <t>0.1215</t>
-  </si>
-  <si>
-    <t>0.1129</t>
-  </si>
-  <si>
-    <t>0.1131</t>
-  </si>
-  <si>
-    <t>0.1130</t>
+    <t>Tempo (s)4</t>
   </si>
 </sst>
 </file>
@@ -296,7 +272,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -315,27 +291,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -404,17 +360,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -425,89 +370,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,7 +554,7 @@
     <tableColumn id="2" xr3:uid="{BEE67F5F-639F-4198-8923-C968C912BD44}" name="Tempo (s)" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{D5B84620-3572-4914-A4F7-0370118E7438}" name="Medidas2" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{5DB27C60-0841-4942-8D89-EE6F9B3ACBE8}" name="Tempo (s)3" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{2170E6E5-AEE3-4290-A90D-DDDFFE888FCB}" name="Medidas4" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2170E6E5-AEE3-4290-A90D-DDDFFE888FCB}" name="Tempo (s)4" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{9079A233-BE31-4F61-98BB-6E544BC6065B}" name="Tempo (s)5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -930,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B82AAC3-63F6-4324-AB66-93B52360566E}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,385 +874,337 @@
     <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>19</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="23"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>20</v>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="9" t="s">
+      <c r="D5" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="10" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="9" t="s">
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="11" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="17"/>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="D14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="9" t="s">
+      <c r="B15" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="9" t="s">
+      <c r="D15" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="10" t="s">
+      <c r="C20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="9" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="11" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="4"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="14"/>
       <c r="D24" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="7" t="s">
-        <v>64</v>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="A1:D2"/>
     <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="A20:A24"/>
     <mergeCell ref="C15:C19"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="C5:C9"/>
-    <mergeCell ref="E5:E9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="E10:E14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>